<commit_message>
a little code cleaning
</commit_message>
<xml_diff>
--- a/Data/model_outputs_baseline/energy/total_carbon_emissions.xlsx
+++ b/Data/model_outputs_baseline/energy/total_carbon_emissions.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>765740476.9219801</v>
+        <v>766036161.559076</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>764843186.4364431</v>
+        <v>765399909.6470771</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>764609265.3743387</v>
+        <v>765397230.966552</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>764116034.7593992</v>
+        <v>765108571.0821869</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>763665758.8846014</v>
+        <v>764839221.7806975</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>763254340.0535032</v>
+        <v>764588093.9251032</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>762878772.9288357</v>
+        <v>764354114.6081029</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>762535848.291002</v>
+        <v>764136780.0966395</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>762222789.9069825</v>
+        <v>763934997.3329364</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>761937775.6888713</v>
+        <v>763748858.7878906</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>761678426.3164039</v>
+        <v>763577215.6567816</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>761442904.7528056</v>
+        <v>763419705.5346628</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>761230095.7392559</v>
+        <v>763275878.5058975</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>761038480.4102097</v>
+        <v>763145252.7714658</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>760867027.3131022</v>
+        <v>763027796.5122873</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>760714382.2106346</v>
+        <v>762923022.9448738</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>760579397.3011948</v>
+        <v>762830588.7212307</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>760461745.4258268</v>
+        <v>762750677.5739375</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>760360692.8796766</v>
+        <v>762682915.3904371</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>760275877.6400875</v>
+        <v>762627321.3109396</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>760206609.0927271</v>
+        <v>762583504.5762452</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>760152511.762825</v>
+        <v>762551444.4014587</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>760112895.2932515</v>
+        <v>762531091.9200835</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>760087575.7310058</v>
+        <v>762522539.0934955</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>760075735.4967388</v>
+        <v>762525265.1644193</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>760077838.6030378</v>
+        <v>762540167.1498311</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>760093050.1396116</v>
+        <v>762566407.9186606</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>760121671.9186164</v>
+        <v>762604424.5888826</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>760163421.7397779</v>
+        <v>762654157.7739567</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>760217905.9869115</v>
+        <v>762715425.5824053</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>760285198.7060713</v>
+        <v>762788307.2760644</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>760365130.6001272</v>
+        <v>762872775.4235002</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>760457532.5755628</v>
+        <v>762968870.2014166</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>760562631.817347</v>
+        <v>763076822.4765112</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>760680261.5341693</v>
+        <v>763196459.4090859</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>760810743.7408731</v>
+        <v>763328320.2027167</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>760953263.1613299</v>
+        <v>763471592.3425705</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>761108423.3138252</v>
+        <v>763626862.5512784</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>761275690.2711564</v>
+        <v>763793774.0245078</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>761455744.2604222</v>
+        <v>763972989.5505404</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>761648159.0143725</v>
+        <v>764164085.009802</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>761853298.775001</v>
+        <v>764367494.0942149</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>762070651.4248791</v>
+        <v>764582773.7272007</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>762300569.573194</v>
+        <v>764810278.0519987</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>762542819.8976628</v>
+        <v>765049775.2803804</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>762797753.1802622</v>
+        <v>765301684.6215496</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>763065479.0302738</v>
+        <v>765566116.9120299</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>763345569.5417149</v>
+        <v>765842645.4730819</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>763638365.1401068</v>
+        <v>766131611.9574701</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>763943556.5209069</v>
+        <v>766432774.7719874</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>764261659.0916926</v>
+        <v>766746583.8628201</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>764592679.173757</v>
+        <v>767073113.0580568</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>764936249.1293494</v>
+        <v>767411995.6403792</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>765292243.506297</v>
+        <v>767763173.1530589</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>765661230.520623</v>
+        <v>768127016.5075139</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>766043280.0548725</v>
+        <v>768503794.731758</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>766437932.0583405</v>
+        <v>768892982.6205065</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>766845255.6316593</v>
+        <v>769294781.5266857</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>767265914.7345538</v>
+        <v>769709659.025849</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>767699265.9019731</v>
+        <v>770137038.341578</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>768145441.2404478</v>
+        <v>770577117.8599564</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>768604682.8245367</v>
+        <v>771030075.0123146</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>769077174.8526102</v>
+        <v>771496160.072034</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>769562270.5457249</v>
+        <v>771974661.8214843</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>770060495.8399401</v>
+        <v>772466107.117155</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>770572096.7974176</v>
+        <v>772970742.9416411</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>771096230.7189692</v>
+        <v>773487792.2616858</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>771633702.6732128</v>
+        <v>774017931.4730695</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>772184543.2558928</v>
+        <v>774561321.4806978</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>772748019.6647633</v>
+        <v>775117101.2185688</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>773325227.1912855</v>
+        <v>775686431.5418041</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>773915055.7435212</v>
+        <v>776268267.5130461</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>774518464.5583731</v>
+        <v>776863504.8509414</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>775135112.128233</v>
+        <v>777471802.9683133</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>775764789.2283615</v>
+        <v>778092889.6335183</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>776407862.4825699</v>
+        <v>778727196.5226759</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>777064057.5375757</v>
+        <v>779374450.2029365</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>777733975.1961838</v>
+        <v>780035188.7770107</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>778416980.015435</v>
+        <v>780708841.5474375</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>779113644.5798479</v>
+        <v>781396045.4351544</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>779823609.2311002</v>
+        <v>782096251.4543127</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>780547221.1570917</v>
+        <v>782809871.5383112</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>781284099.044209</v>
+        <v>783536588.7099549</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>782034886.2962449</v>
+        <v>784277047.2934682</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>782799186.7241476</v>
+        <v>785030717.2123425</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>783577602.2766207</v>
+        <v>785798336.5819434</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>784369432.9552692</v>
+        <v>786579080.924118</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>785175573.071694</v>
+        <v>787373908.6823466</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>785995473.7113369</v>
+        <v>788182272.1693126</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>786829784.4305093</v>
+        <v>789004822.16857</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>787677897.4946395</v>
+        <v>789840952.1727909</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>788540572.6251842</v>
+        <v>790691485.3194181</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>789417698.9273072</v>
+        <v>791556249.5475727</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>790309206.0712463</v>
+        <v>792435175.7547365</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>791215959.8313591</v>
+        <v>793329069.0605773</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>792137108.5044324</v>
+        <v>794237079.2959349</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>793073375.62249</v>
+        <v>795159931.5268861</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>794025083.0178366</v>
+        <v>796098072.2700338</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>794992188.164067</v>
+        <v>797051336.973701</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>795974844.7407006</v>
+        <v>798019942.2220426</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>796973584.8345106</v>
+        <v>799004360.060762</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>797988054.2043717</v>
+        <v>800004298.9488297</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>799018984.0186512</v>
+        <v>801020491.2818553</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>800066792.1170353</v>
+        <v>802053295.1652663</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>801130977.9989058</v>
+        <v>803102229.2103695</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>802212784.8669724</v>
+        <v>804168563.7256083</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>803311952.1505485</v>
+        <v>805252056.9749478</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>804428947.2141255</v>
+        <v>806353116.9977027</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>805563842.2315201</v>
+        <v>807471808.8542423</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>806717487.1527978</v>
+        <v>808608992.7054455</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>807890223.9003059</v>
+        <v>809765072.2533227</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>809081912.8295367</v>
+        <v>810939848.9372706</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>810293359.0288429</v>
+        <v>812134189.420763</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>811525357.3900044</v>
+        <v>813348889.8228228</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>812777698.5364616</v>
+        <v>814583682.1576053</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>814050681.3709962</v>
+        <v>815838926.5962037</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>815345502.0215279</v>
+        <v>817115820.4937797</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>816662623.8950702</v>
+        <v>818414828.4845901</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>818002217.0776765</v>
+        <v>819736121.8819309</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>819364695.5242187</v>
+        <v>821080056.54274</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>820750973.5476282</v>
+        <v>822447607.5369087</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>822161481.2280648</v>
+        <v>823839206.1718394</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>823597300.6502445</v>
+        <v>825255935.7594916</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>825057816.1689429</v>
+        <v>826697240.7979788</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>826545276.7281513</v>
+        <v>828165312.3378989</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>828059236.2163476</v>
+        <v>829659772.6053201</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>829601013.6810662</v>
+        <v>831181933.1401577</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>831170428.2702506</v>
+        <v>832731555.5037711</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>832769316.4957823</v>
+        <v>834310535.84003</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>834397627.1295176</v>
+        <v>835918823.8412228</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>836056649.3136414</v>
+        <v>837557651.3697613</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>837746362.672014</v>
+        <v>839227049.0636715</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>839468750.6637063</v>
+        <v>840929009.6427275</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>841223598.2104913</v>
+        <v>842663318.9491352</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>843012283.9182014</v>
+        <v>844431356.5091593</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>844835093.7635785</v>
+        <v>846233466.9088259</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>846693952.638275</v>
+        <v>848071575.6534097</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>848588312.4853477</v>
+        <v>849945077.8152759</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>850520235.869579</v>
+        <v>851856094.2616812</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>852490054.6503789</v>
+        <v>853804957.4656576</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>854499056.9067577</v>
+        <v>855793013.2973384</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>856547062.1810045</v>
+        <v>857820024.5305921</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>858636877.823867</v>
+        <v>859888856.1027484</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>860767958.3727725</v>
+        <v>861998905.9873551</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>862941900.7742076</v>
+        <v>864151828.5129409</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>865159366.6238124</v>
+        <v>866348285.5819561</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>867422225.5238051</v>
+        <v>868590147.1034298</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>869729929.7833983</v>
+        <v>870876865.6933864</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>872085136.1983855</v>
+        <v>873211098.4544283</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>874487536.8150637</v>
+        <v>875592650.2538049</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>876938875.5453526</v>
+        <v>878023208.5418245</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>879439919.8361796</v>
+        <v>880503484.7128856</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>881991932.5285175</v>
+        <v>883034853.8152897</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>884595644.6040826</v>
+        <v>885617990.6759536</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>887252742.7207001</v>
+        <v>888254581.9527026</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>889963062.352132</v>
+        <v>890944518.7627474</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>892728535.0112112</v>
+        <v>893689732.3121103</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>895549805.4721935</v>
+        <v>896490811.6293278</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>898428789.1558216</v>
+        <v>899349782.808419</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>901365702.2587479</v>
+        <v>902266806.1980474</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>904362022.6041752</v>
+        <v>905243359.3146044</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>907418543.9807379</v>
+        <v>908280290.6697416</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>910536667.1797379</v>
+        <v>911379000.4411397</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>913717343.4091351</v>
+        <v>914540439.2231367</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>916961376.9870715</v>
+        <v>917765410.7202533</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>920269931.1882219</v>
+        <v>921055077.5935436</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>923644642.8885186</v>
+        <v>924411021.5868416</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>927085290.5083716</v>
+        <v>927833129.6461587</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>930594541.0805142</v>
+        <v>931324013.6564814</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>934172026.0634117</v>
+        <v>934883412.7123883</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>937820073.1811165</v>
+        <v>938513491.1553891</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>941538132.2258397</v>
+        <v>942213860.4056393</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>945329230.320925</v>
+        <v>945987492.3691839</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>949192313.6817346</v>
+        <v>949833278.7091248</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>953130411.8163549</v>
+        <v>953754409.2508242</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>957142623.015885</v>
+        <v>957749820.1265317</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>961232127.8325933</v>
+        <v>961822798.0978153</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>965397523.461174</v>
+        <v>965971885.9065393</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>969642182.5426234</v>
+        <v>970200508.3972956</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>973964984.2281321</v>
+        <v>974507604.4582663</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>978369004.9746306</v>
+        <v>978896188.285966</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>982853138.7661849</v>
+        <v>983365152.4732833</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>987420715.6144035</v>
+        <v>987917825.9678133</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>992070267.9948329</v>
+        <v>992552687.0754532</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>996805169.3744124</v>
+        <v>997273161.1821413</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>1001624561.996832</v>
+        <v>1002078389.143211</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>1006530747.01637</v>
+        <v>1006970723.519179</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>1011523426.037086</v>
+        <v>1011949811.849545</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>1016605174.02397</v>
+        <v>1017018280.299587</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>1021775280.122634</v>
+        <v>1022175364.077143</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>1027036417.716789</v>
+        <v>1027423676.064855</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>1032387955.002316</v>
+        <v>1032762702.370325</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>1037832368.840321</v>
+        <v>1038194799.797153</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>1043369253.443924</v>
+        <v>1043719672.289274</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>1049000992.948353</v>
+        <v>1049339761.724258</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>1054727598.541264</v>
+        <v>1055054907.768189</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>1060550243.30705</v>
+        <v>1060866393.119758</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>1066470174.335593</v>
+        <v>1066775470.678649</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>1072488535.588951</v>
+        <v>1072783216.69519</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>1078605615.813677</v>
+        <v>1078889926.275626</v>
       </c>
     </row>
     <row r="202">
@@ -2043,7 +2043,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>1084823370.337017</v>
+        <v>1085097611.861222</v>
       </c>
     </row>
     <row r="203">
@@ -2051,7 +2051,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>1091142439.00944</v>
+        <v>1091406795.345981</v>
       </c>
     </row>
     <row r="204">
@@ -2059,7 +2059,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>1097563495.957516</v>
+        <v>1097818309.39169</v>
       </c>
     </row>
     <row r="205">
@@ -2067,7 +2067,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>1104088067.002391</v>
+        <v>1104333634.798184</v>
       </c>
     </row>
     <row r="206">
@@ -2075,7 +2075,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>1110717079.168869</v>
+        <v>1110953530.701936</v>
       </c>
     </row>
     <row r="207">
@@ -2083,7 +2083,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>1117451473.701097</v>
+        <v>1117679096.230067</v>
       </c>
     </row>
     <row r="208">
@@ -2091,7 +2091,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>1124292575.218256</v>
+        <v>1124511712.401303</v>
       </c>
     </row>
     <row r="209">
@@ -2099,7 +2099,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>1131241408.971714</v>
+        <v>1131452186.953628</v>
       </c>
     </row>
     <row r="210">
@@ -2107,7 +2107,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>1138298981.359587</v>
+        <v>1138501790.839834</v>
       </c>
     </row>
     <row r="211">
@@ -2115,7 +2115,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>1145466131.310346</v>
+        <v>1145661153.431484</v>
       </c>
     </row>
     <row r="212">
@@ -2123,7 +2123,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>1152744569.999485</v>
+        <v>1152932092.174522</v>
       </c>
     </row>
     <row r="213">
@@ -2131,7 +2131,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>1160135269.546921</v>
+        <v>1160315463.214995</v>
       </c>
     </row>
     <row r="214">
@@ -2139,7 +2139,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>1167639253.990006</v>
+        <v>1167812346.937484</v>
       </c>
     </row>
     <row r="215">
@@ -2147,7 +2147,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>1175257982.239471</v>
+        <v>1175424201.023936</v>
       </c>
     </row>
     <row r="216">
@@ -2155,7 +2155,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>1182992473.864736</v>
+        <v>1183152100.521232</v>
       </c>
     </row>
     <row r="217">
@@ -2163,7 +2163,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>1190843898.128958</v>
+        <v>1190997050.497109</v>
       </c>
     </row>
     <row r="218">
@@ -2171,7 +2171,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>1198813928.198882</v>
+        <v>1198960878.41754</v>
       </c>
     </row>
     <row r="219">
@@ -2179,7 +2179,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>1206903476.804369</v>
+        <v>1207044446.520744</v>
       </c>
     </row>
     <row r="220">
@@ -2187,7 +2187,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>1215113866.912553</v>
+        <v>1215249083.583303</v>
       </c>
     </row>
     <row r="221">
@@ -2195,7 +2195,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>1223446640.239618</v>
+        <v>1223576266.971972</v>
       </c>
     </row>
     <row r="222">
@@ -2203,7 +2203,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>1231903363.612301</v>
+        <v>1232027618.236766</v>
       </c>
     </row>
     <row r="223">
@@ -2211,7 +2211,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>1240484682.575485</v>
+        <v>1240603733.139827</v>
       </c>
     </row>
     <row r="224">
@@ -2219,7 +2219,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>1249192656.671125</v>
+        <v>1249306726.072201</v>
       </c>
     </row>
     <row r="225">
@@ -2227,7 +2227,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>1258028718.317027</v>
+        <v>1258137916.937902</v>
       </c>
     </row>
     <row r="226">
@@ -2235,7 +2235,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>1266993980.861696</v>
+        <v>1267098522.243121</v>
       </c>
     </row>
     <row r="227">
@@ -2243,7 +2243,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>1276090508.251805</v>
+        <v>1276190556.553874</v>
       </c>
     </row>
     <row r="228">
@@ -2251,7 +2251,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>1285319494.75577</v>
+        <v>1285415261.598915</v>
       </c>
     </row>
     <row r="229">
@@ -2259,7 +2259,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>1294682891.70802</v>
+        <v>1294774546.110489</v>
       </c>
     </row>
     <row r="230">
@@ -2267,7 +2267,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>1304181247.463194</v>
+        <v>1304268895.581226</v>
       </c>
     </row>
     <row r="231">
@@ -2275,7 +2275,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>1313818106.82004</v>
+        <v>1313901908.744422</v>
       </c>
     </row>
     <row r="232">
@@ -2283,7 +2283,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>1323593801.135093</v>
+        <v>1323673916.42201</v>
       </c>
     </row>
     <row r="233">
@@ -2291,7 +2291,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>1333510380.375167</v>
+        <v>1333586919.787976</v>
       </c>
     </row>
     <row r="234">
@@ -2299,7 +2299,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>1343569695.412539</v>
+        <v>1343642816.868144</v>
       </c>
     </row>
     <row r="235">
@@ -2307,7 +2307,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>1353774205.758197</v>
+        <v>1353844120.736742</v>
       </c>
     </row>
     <row r="236">
@@ -2315,7 +2315,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>1364124528.879547</v>
+        <v>1364191290.917923</v>
       </c>
     </row>
     <row r="237">
@@ -2323,7 +2323,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>1374623629.346509</v>
+        <v>1374687393.807206</v>
       </c>
     </row>
     <row r="238">
@@ -2331,7 +2331,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>1385273522.288066</v>
+        <v>1385334396.252098</v>
       </c>
     </row>
     <row r="239">
@@ -2339,7 +2339,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>1396075332.013949</v>
+        <v>1396133469.204526</v>
       </c>
     </row>
     <row r="240">
@@ -2347,7 +2347,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>1407032370.800395</v>
+        <v>1407087883.609427</v>
       </c>
     </row>
     <row r="241">
@@ -2355,7 +2355,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>1418146108.326098</v>
+        <v>1418199048.033249</v>
       </c>
     </row>
     <row r="242">
@@ -2363,7 +2363,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>1429418560.442659</v>
+        <v>1429469078.260357</v>
       </c>
     </row>
     <row r="243">
@@ -2371,7 +2371,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>1440852006.521636</v>
+        <v>1440900259.806426</v>
       </c>
     </row>
     <row r="244">
@@ -2379,7 +2379,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>1452449963.021533</v>
+        <v>1452496054.73115</v>
       </c>
     </row>
     <row r="245">
@@ -2387,7 +2387,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>1464212908.32287</v>
+        <v>1464256940.79998</v>
       </c>
     </row>
     <row r="246">
@@ -2395,7 +2395,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>1476144945.981583</v>
+        <v>1476186974.412403</v>
       </c>
     </row>
     <row r="247">
@@ -2403,7 +2403,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>1488247453.380052</v>
+        <v>1488287579.081696</v>
       </c>
     </row>
     <row r="248">
@@ -2411,7 +2411,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>1500523908.471438</v>
+        <v>1500562278.081522</v>
       </c>
     </row>
     <row r="249">
@@ -2419,7 +2419,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>1512976021.298454</v>
+        <v>1513012688.472483</v>
       </c>
     </row>
     <row r="250">
@@ -2427,7 +2427,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>1525607177.209488</v>
+        <v>1525642241.427017</v>
       </c>
     </row>
     <row r="251">
@@ -2435,7 +2435,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>1538419847.957148</v>
+        <v>1538453362.052621</v>
       </c>
     </row>
     <row r="252">
@@ -2443,7 +2443,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>1551416472.633828</v>
+        <v>1551448489.13345</v>
       </c>
     </row>
     <row r="253">
@@ -2451,7 +2451,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>1564601188.14079</v>
+        <v>1564631805.088045</v>
       </c>
     </row>
     <row r="254">
@@ -2459,7 +2459,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>1577975523.911104</v>
+        <v>1578004793.011218</v>
       </c>
     </row>
     <row r="255">
@@ -2467,7 +2467,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>1591543465.840082</v>
+        <v>1591571438.105674</v>
       </c>
     </row>
     <row r="256">
@@ -2475,7 +2475,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>1605307678.476886</v>
+        <v>1605334450.522932</v>
       </c>
     </row>
     <row r="257">
@@ -2483,7 +2483,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>1619271933.132427</v>
+        <v>1619297555.542418</v>
       </c>
     </row>
     <row r="258">
@@ -2491,7 +2491,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>1633438298.305544</v>
+        <v>1633462821.354734</v>
       </c>
     </row>
     <row r="259">
@@ -2499,7 +2499,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>1647811640.440929</v>
+        <v>1647835159.308236</v>
       </c>
     </row>
     <row r="260">
@@ -2507,7 +2507,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>1662394331.161507</v>
+        <v>1662416850.191596</v>
       </c>
     </row>
     <row r="261">
@@ -2515,7 +2515,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>1677190382.264134</v>
+        <v>1677211995.814976</v>
       </c>
     </row>
     <row r="262">
@@ -2523,7 +2523,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>1692203029.285775</v>
+        <v>1692223785.773827</v>
       </c>
     </row>
     <row r="263">
@@ -2531,7 +2531,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="n">
-        <v>1707436041.436577</v>
+        <v>1707455989.399978</v>
       </c>
     </row>
     <row r="264">
@@ -2539,7 +2539,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="n">
-        <v>1722893721.894276</v>
+        <v>1722912864.862386</v>
       </c>
     </row>
     <row r="265">
@@ -2547,7 +2547,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="n">
-        <v>1738578889.0879</v>
+        <v>1738597275.186923</v>
       </c>
     </row>
     <row r="266">
@@ -2555,7 +2555,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="n">
-        <v>1754496911.740634</v>
+        <v>1754514544.292563</v>
       </c>
     </row>
     <row r="267">
@@ -2563,7 +2563,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="n">
-        <v>1770650283.171007</v>
+        <v>1770667254.28389</v>
       </c>
     </row>
     <row r="268">
@@ -2571,7 +2571,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="n">
-        <v>1787044299.167193</v>
+        <v>1787060656.042621</v>
       </c>
     </row>
     <row r="269">
@@ -2579,7 +2579,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>1803682672.890456</v>
+        <v>1803698418.232661</v>
       </c>
     </row>
     <row r="270">
@@ -2587,7 +2587,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>1820570271.75868</v>
+        <v>1820585452.357453</v>
       </c>
     </row>
     <row r="271">
@@ -2595,7 +2595,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>1837710487.301972</v>
+        <v>1837725193.179048</v>
       </c>
     </row>
     <row r="272">
@@ -2603,7 +2603,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>1855109208.102499</v>
+        <v>1855123305.612838</v>
       </c>
     </row>
     <row r="273">
@@ -2611,7 +2611,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>1872769711.900514</v>
+        <v>1872783343.429055</v>
       </c>
     </row>
     <row r="274">
@@ -2619,7 +2619,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="n">
-        <v>1890697531.166213</v>
+        <v>1890710694.610714</v>
       </c>
     </row>
     <row r="275">
@@ -2627,7 +2627,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="n">
-        <v>1908897253.465574</v>
+        <v>1908909950.916631</v>
       </c>
     </row>
     <row r="276">
@@ -2635,7 +2635,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="n">
-        <v>1927373603.399766</v>
+        <v>1927385880.419904</v>
       </c>
     </row>
     <row r="277">
@@ -2643,7 +2643,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="n">
-        <v>1946131779.460938</v>
+        <v>1946143681.304521</v>
       </c>
     </row>
     <row r="278">
@@ -2651,7 +2651,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="n">
-        <v>1965177460.971099</v>
+        <v>1965188989.315597</v>
       </c>
     </row>
     <row r="279">
@@ -2659,7 +2659,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="n">
-        <v>1984515203.434797</v>
+        <v>1984526402.70316</v>
       </c>
     </row>
     <row r="280">
@@ -2667,7 +2667,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="n">
-        <v>2004150216.406149</v>
+        <v>2004161088.030161</v>
       </c>
     </row>
     <row r="281">
@@ -2675,7 +2675,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="n">
-        <v>2024089092.38973</v>
+        <v>2024099597.821859</v>
       </c>
     </row>
     <row r="282">
@@ -2683,7 +2683,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="n">
-        <v>2044335786.081261</v>
+        <v>2044345921.537376</v>
       </c>
     </row>
     <row r="283">
@@ -2691,7 +2691,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="n">
-        <v>2064897488.35146</v>
+        <v>2064907333.994111</v>
       </c>
     </row>
     <row r="284">
@@ -2699,7 +2699,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="n">
-        <v>2085778822.947139</v>
+        <v>2085788436.579163</v>
       </c>
     </row>
     <row r="285">
@@ -2707,7 +2707,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="n">
-        <v>2106986030.567373</v>
+        <v>2106995285.715501</v>
       </c>
     </row>
     <row r="286">
@@ -2715,7 +2715,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="n">
-        <v>2128525756.214144</v>
+        <v>2128534811.733783</v>
       </c>
     </row>
     <row r="287">
@@ -2723,7 +2723,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="n">
-        <v>2150403315.79034</v>
+        <v>2150412108.222808</v>
       </c>
     </row>
     <row r="288">
@@ -2731,7 +2731,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="n">
-        <v>2172625228.031062</v>
+        <v>2172633788.684901</v>
       </c>
     </row>
     <row r="289">
@@ -2739,7 +2739,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="n">
-        <v>2195197497.510647</v>
+        <v>2195205911.343991</v>
       </c>
     </row>
     <row r="290">
@@ -2747,7 +2747,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="n">
-        <v>2218127399.150997</v>
+        <v>2218135620.94346</v>
       </c>
     </row>
     <row r="291">
@@ -2755,7 +2755,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="n">
-        <v>2241420568.101599</v>
+        <v>2241428714.900163</v>
       </c>
     </row>
     <row r="292">
@@ -2763,7 +2763,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="n">
-        <v>2265084936.468368</v>
+        <v>2265092954.578098</v>
       </c>
     </row>
     <row r="293">
@@ -2771,7 +2771,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="n">
-        <v>2289125640.263159</v>
+        <v>2289133506.449254</v>
       </c>
     </row>
     <row r="294">
@@ -2779,7 +2779,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="n">
-        <v>2313551069.270512</v>
+        <v>2313558676.316206</v>
       </c>
     </row>
     <row r="295">
@@ -2787,7 +2787,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="n">
-        <v>2338367187.405917</v>
+        <v>2338374574.723897</v>
       </c>
     </row>
     <row r="296">
@@ -2795,7 +2795,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="n">
-        <v>2363581772.813383</v>
+        <v>2363588812.618381</v>
       </c>
     </row>
     <row r="297">
@@ -2803,7 +2803,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="n">
-        <v>2389201852.577587</v>
+        <v>2389208579.465167</v>
       </c>
     </row>
     <row r="298">
@@ -2811,7 +2811,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="n">
-        <v>2415234391.443898</v>
+        <v>2415240844.174005</v>
       </c>
     </row>
     <row r="299">
@@ -2819,7 +2819,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="n">
-        <v>2441687094.263894</v>
+        <v>2441693162.502462</v>
       </c>
     </row>
     <row r="300">
@@ -2827,7 +2827,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="n">
-        <v>2468567823.898155</v>
+        <v>2468573566.389735</v>
       </c>
     </row>
     <row r="301">
@@ -2835,7 +2835,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="n">
-        <v>2495883197.330089</v>
+        <v>2495888601.210467</v>
       </c>
     </row>
     <row r="302">
@@ -2843,7 +2843,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="n">
-        <v>2523642083.654566</v>
+        <v>2523647270.470092</v>
       </c>
     </row>
     <row r="303">
@@ -2851,7 +2851,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="n">
-        <v>2546397472.046915</v>
+        <v>2546402285.277782</v>
       </c>
     </row>
     <row r="304">
@@ -2859,7 +2859,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="n">
-        <v>2569543287.382156</v>
+        <v>2569547873.645792</v>
       </c>
     </row>
     <row r="305">
@@ -2867,7 +2867,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="n">
-        <v>2593084446.175806</v>
+        <v>2593088727.06467</v>
       </c>
     </row>
     <row r="306">
@@ -2875,7 +2875,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="n">
-        <v>2617028132.135296</v>
+        <v>2617032072.207896</v>
       </c>
     </row>
     <row r="307">
@@ -2883,7 +2883,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="n">
-        <v>2641382348.294893</v>
+        <v>2641386152.220503</v>
       </c>
     </row>
     <row r="308">
@@ -2891,7 +2891,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="n">
-        <v>2666153291.645896</v>
+        <v>2666156845.597673</v>
       </c>
     </row>
     <row r="309">
@@ -2899,7 +2899,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="n">
-        <v>2691348853.200941</v>
+        <v>2691352259.523121</v>
       </c>
     </row>
     <row r="310">
@@ -2907,7 +2907,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="n">
-        <v>2716975209.170382</v>
+        <v>2716978331.452926</v>
       </c>
     </row>
     <row r="311">
@@ -2915,7 +2915,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="n">
-        <v>2743040211.530872</v>
+        <v>2743043174.987037</v>
       </c>
     </row>
     <row r="312">
@@ -2923,7 +2923,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="n">
-        <v>2769550897.640516</v>
+        <v>2769553801.706634</v>
       </c>
     </row>
     <row r="313">
@@ -2931,7 +2931,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>2796514618.466906</v>
+        <v>2796517398.502613</v>
       </c>
     </row>
     <row r="314">
@@ -2939,7 +2939,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="n">
-        <v>2823938903.10076</v>
+        <v>2823941523.446121</v>
       </c>
     </row>
     <row r="315">
@@ -2947,7 +2947,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="n">
-        <v>2851830376.185478</v>
+        <v>2851832819.708213</v>
       </c>
     </row>
     <row r="316">
@@ -2955,7 +2955,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="n">
-        <v>2880196447.792754</v>
+        <v>2880198801.156144</v>
       </c>
     </row>
     <row r="317">
@@ -2963,7 +2963,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="n">
-        <v>2909045757.756967</v>
+        <v>2909047990.427411</v>
       </c>
     </row>
     <row r="318">
@@ -2971,7 +2971,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="n">
-        <v>2938383840.199207</v>
+        <v>2938385887.024764</v>
       </c>
     </row>
     <row r="319">
@@ -2979,7 +2979,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="n">
-        <v>2968219286.962169</v>
+        <v>2968221287.761933</v>
       </c>
     </row>
     <row r="320">
@@ -2987,7 +2987,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>2998558982.814799</v>
+        <v>2998560845.225222</v>
       </c>
     </row>
     <row r="321">
@@ -2995,7 +2995,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>3029409688.546867</v>
+        <v>3029411454.854049</v>
       </c>
     </row>
     <row r="322">
@@ -3003,7 +3003,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="n">
-        <v>3060779347.666999</v>
+        <v>3060780879.344106</v>
       </c>
     </row>
     <row r="323">
@@ -3011,7 +3011,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="n">
-        <v>3092675077.941347</v>
+        <v>3092676557.836377</v>
       </c>
     </row>
     <row r="324">
@@ -3019,7 +3019,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="n">
-        <v>3125103860.368706</v>
+        <v>3125105300.701602</v>
       </c>
     </row>
     <row r="325">
@@ -3027,7 +3027,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="n">
-        <v>3158073028.755718</v>
+        <v>3158074463.069406</v>
       </c>
     </row>
     <row r="326">
@@ -3035,7 +3035,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="n">
-        <v>3191589094.597942</v>
+        <v>3191590459.382695</v>
       </c>
     </row>
     <row r="327">
@@ -3043,7 +3043,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="n">
-        <v>3225659360.297003</v>
+        <v>3225660534.810781</v>
       </c>
     </row>
     <row r="328">
@@ -3051,7 +3051,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="n">
-        <v>3260290591.184377</v>
+        <v>3260291673.361605</v>
       </c>
     </row>
     <row r="329">
@@ -3059,7 +3059,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="n">
-        <v>3295489635.513497</v>
+        <v>3295490671.003623</v>
       </c>
     </row>
     <row r="330">
@@ -3067,7 +3067,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>3331262975.617246</v>
+        <v>3331264009.282507</v>
       </c>
     </row>
     <row r="331">
@@ -3075,7 +3075,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>3367617079.691375</v>
+        <v>3367618080.520342</v>
       </c>
     </row>
     <row r="332">
@@ -3083,7 +3083,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="n">
-        <v>3404558373.184359</v>
+        <v>3404559317.053241</v>
       </c>
     </row>
     <row r="333">
@@ -3091,7 +3091,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="n">
-        <v>3442092606.015641</v>
+        <v>3442093511.301157</v>
       </c>
     </row>
     <row r="334">
@@ -3099,7 +3099,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="n">
-        <v>3480226147.692998</v>
+        <v>3480227010.174866</v>
       </c>
     </row>
     <row r="335">
@@ -3107,7 +3107,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="n">
-        <v>3518964930.47512</v>
+        <v>3518965705.208033</v>
       </c>
     </row>
     <row r="336">
@@ -3115,7 +3115,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="n">
-        <v>3558314180.332041</v>
+        <v>3558314922.15642</v>
       </c>
     </row>
     <row r="337">
@@ -3123,7 +3123,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="n">
-        <v>3598279983.229684</v>
+        <v>3598280681.107358</v>
       </c>
     </row>
     <row r="338">
@@ -3131,7 +3131,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="n">
-        <v>3638866587.441125</v>
+        <v>3638867221.895248</v>
       </c>
     </row>
     <row r="339">
@@ -3139,7 +3139,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="n">
-        <v>3680079234.072449</v>
+        <v>3680079771.018334</v>
       </c>
     </row>
     <row r="340">
@@ -3147,7 +3147,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="n">
-        <v>3721922766.856763</v>
+        <v>3721923302.380811</v>
       </c>
     </row>
     <row r="341">
@@ -3155,7 +3155,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="n">
-        <v>3764401660.075916</v>
+        <v>3764402194.178126</v>
       </c>
     </row>
     <row r="342">
@@ -3163,7 +3163,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="n">
-        <v>3807519473.998374</v>
+        <v>3807520010.609378</v>
       </c>
     </row>
     <row r="343">
@@ -3171,7 +3171,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="n">
-        <v>3851280574.441673</v>
+        <v>3851281117.183795</v>
       </c>
     </row>
     <row r="344">
@@ -3179,7 +3179,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="n">
-        <v>3895688606.771215</v>
+        <v>3895689154.48123</v>
       </c>
     </row>
     <row r="345">
@@ -3187,7 +3187,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>3940745886.240779</v>
+        <v>3940746303.192792</v>
       </c>
     </row>
     <row r="346">
@@ -3195,7 +3195,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="n">
-        <v>3986455775.153798</v>
+        <v>3986456150.313171</v>
       </c>
     </row>
     <row r="347">
@@ -3203,7 +3203,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="n">
-        <v>4032820624.639124</v>
+        <v>4032821006.910999</v>
       </c>
     </row>
     <row r="348">
@@ -3211,7 +3211,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="n">
-        <v>4079842563.772415</v>
+        <v>4079842945.012146</v>
       </c>
     </row>
     <row r="349">
@@ -3219,7 +3219,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="n">
-        <v>4127522864.275818</v>
+        <v>4127523208.322467</v>
       </c>
     </row>
     <row r="350">
@@ -3227,7 +3227,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="n">
-        <v>4175863633.140585</v>
+        <v>4175863935.975323</v>
       </c>
     </row>
     <row r="351">
@@ -3235,7 +3235,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="n">
-        <v>4224864606.123468</v>
+        <v>4224864851.638452</v>
       </c>
     </row>
     <row r="352">
@@ -3243,7 +3243,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="n">
-        <v>4274526918.171777</v>
+        <v>4274527163.014488</v>
       </c>
     </row>
     <row r="353">
@@ -3251,7 +3251,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="n">
-        <v>4324849825.345849</v>
+        <v>4324850069.516289</v>
       </c>
     </row>
     <row r="354">
@@ -3259,7 +3259,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="n">
-        <v>4375833875.826747</v>
+        <v>4375834100.33983</v>
       </c>
     </row>
     <row r="355">
@@ -3267,7 +3267,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="n">
-        <v>4427477144.238274</v>
+        <v>4427477368.130664</v>
       </c>
     </row>
     <row r="356">
@@ -3275,7 +3275,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="n">
-        <v>4479778228.243418</v>
+        <v>4479778451.515115</v>
       </c>
     </row>
     <row r="357">
@@ -3283,7 +3283,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="n">
-        <v>4532735263.858523</v>
+        <v>4532735486.509526</v>
       </c>
     </row>
     <row r="358">
@@ -3291,7 +3291,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="n">
-        <v>4586232981.440354</v>
+        <v>4586233203.470664</v>
       </c>
     </row>
     <row r="359">
@@ -3299,7 +3299,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="n">
-        <v>4640380445.133926</v>
+        <v>4640380666.543543</v>
       </c>
     </row>
     <row r="360">
@@ -3307,7 +3307,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="n">
-        <v>4695172763.101804</v>
+        <v>4695172983.890726</v>
       </c>
     </row>
     <row r="361">
@@ -3315,7 +3315,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="n">
-        <v>4750607191.60332</v>
+        <v>4750607411.77155</v>
       </c>
     </row>
     <row r="362">
@@ -3323,7 +3323,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>4806678517.063559</v>
+        <v>4806678736.611094</v>
       </c>
     </row>
     <row r="363">
@@ -3331,7 +3331,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="n">
-        <v>4863381628.220149</v>
+        <v>4863381809.874703</v>
       </c>
     </row>
     <row r="364">
@@ -3339,7 +3339,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="n">
-        <v>4920710843.470545</v>
+        <v>4920711024.610874</v>
       </c>
     </row>
     <row r="365">
@@ -3347,7 +3347,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="n">
-        <v>4978659180.702556</v>
+        <v>4978659364.682084</v>
       </c>
     </row>
     <row r="366">
@@ -3355,7 +3355,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="n">
-        <v>5037220623.934645</v>
+        <v>5037220807.390285</v>
       </c>
     </row>
     <row r="367">
@@ -3363,7 +3363,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="n">
-        <v>5096386974.435591</v>
+        <v>5096387157.367343</v>
       </c>
     </row>
     <row r="368">
@@ -3371,7 +3371,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="n">
-        <v>5156150539.110787</v>
+        <v>5156150721.518651</v>
       </c>
     </row>
     <row r="369">
@@ -3379,7 +3379,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="n">
-        <v>5216502329.652038</v>
+        <v>5216502471.111222</v>
       </c>
     </row>
     <row r="370">
@@ -3387,7 +3387,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>5277433285.388597</v>
+        <v>5277433481.030805</v>
       </c>
     </row>
     <row r="371">
@@ -3395,7 +3395,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="n">
-        <v>5338933216.24556</v>
+        <v>5338933411.322731</v>
       </c>
     </row>
     <row r="372">
@@ -3403,7 +3403,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="n">
-        <v>5400992345.923256</v>
+        <v>5400992540.43539</v>
       </c>
     </row>
     <row r="373">
@@ -3411,7 +3411,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="n">
-        <v>5463738989.685047</v>
+        <v>5463739183.632143</v>
       </c>
     </row>
     <row r="374">
@@ -3419,7 +3419,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="n">
-        <v>5527023027.484024</v>
+        <v>5527023220.866084</v>
       </c>
     </row>
     <row r="375">
@@ -3427,7 +3427,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="n">
-        <v>5590831914.939089</v>
+        <v>5590832107.756111</v>
       </c>
     </row>
     <row r="376">
@@ -3435,7 +3435,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="n">
-        <v>5655153012.637063</v>
+        <v>5655153204.889048</v>
       </c>
     </row>
     <row r="377">
@@ -3443,7 +3443,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>5719973248.100572</v>
+        <v>5719973439.787519</v>
       </c>
     </row>
     <row r="378">
@@ -3451,7 +3451,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="n">
-        <v>5785278890.014848</v>
+        <v>5785279081.136759</v>
       </c>
     </row>
     <row r="379">
@@ -3459,7 +3459,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>5850997293.244744</v>
+        <v>5850997483.801618</v>
       </c>
     </row>
     <row r="380">
@@ -3467,7 +3467,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>5916471949.629855</v>
+        <v>5916472139.621691</v>
       </c>
     </row>
     <row r="381">
@@ -3475,7 +3475,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>5980035962.799026</v>
+        <v>5980036152.225826</v>
       </c>
     </row>
     <row r="382">
@@ -3483,7 +3483,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="n">
-        <v>6039731385.712023</v>
+        <v>6039731574.573785</v>
       </c>
     </row>
     <row r="383">
@@ -3491,7 +3491,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="n">
-        <v>6113306275.493183</v>
+        <v>6113306463.789909</v>
       </c>
     </row>
     <row r="384">
@@ -3499,7 +3499,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="n">
-        <v>6181481281.76597</v>
+        <v>6181481469.497658</v>
       </c>
     </row>
     <row r="385">
@@ -3507,7 +3507,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="n">
-        <v>6244802767.167819</v>
+        <v>6244802954.33447</v>
       </c>
     </row>
     <row r="386">
@@ -3515,7 +3515,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="n">
-        <v>6304348456.848358</v>
+        <v>6304348643.449972</v>
       </c>
     </row>
     <row r="387">
@@ -3523,7 +3523,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>6361403427.142289</v>
+        <v>6361403613.178866</v>
       </c>
     </row>
     <row r="388">
@@ -3531,7 +3531,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>6417232013.660148</v>
+        <v>6417232199.131687</v>
       </c>
     </row>
     <row r="389">
@@ -3539,7 +3539,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>6472943917.291657</v>
+        <v>6472944102.198159</v>
       </c>
     </row>
     <row r="390">
@@ -3547,7 +3547,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="n">
-        <v>6529437457.945206</v>
+        <v>6529437642.286671</v>
       </c>
     </row>
     <row r="391">
@@ -3555,7 +3555,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>6587390675.543679</v>
+        <v>6587390859.320107</v>
       </c>
     </row>
     <row r="392">
@@ -3563,7 +3563,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="n">
-        <v>6647279047.736644</v>
+        <v>6647279230.948035</v>
       </c>
     </row>
     <row r="393">
@@ -3571,7 +3571,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="n">
-        <v>6699593241.322508</v>
+        <v>6699593423.968862</v>
       </c>
     </row>
     <row r="394">
@@ -3579,7 +3579,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="n">
-        <v>6754004618.064929</v>
+        <v>6754004800.146246</v>
       </c>
     </row>
     <row r="395">
@@ -3587,7 +3587,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="n">
-        <v>6810619069.024395</v>
+        <v>6810619250.540674</v>
       </c>
     </row>
     <row r="396">
@@ -3595,7 +3595,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="n">
-        <v>6869462230.22877</v>
+        <v>6869462411.180013</v>
       </c>
     </row>
     <row r="397">
@@ -3603,7 +3603,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="n">
-        <v>6930500121.362403</v>
+        <v>6930500301.748608</v>
       </c>
     </row>
     <row r="398">
@@ -3611,7 +3611,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="n">
-        <v>6993657411.086907</v>
+        <v>6993657590.908074</v>
       </c>
     </row>
     <row r="399">
@@ -3619,7 +3619,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="n">
-        <v>7058828293.428326</v>
+        <v>7058575963.639893</v>
       </c>
     </row>
     <row r="400">
@@ -3627,7 +3627,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="n">
-        <v>7125889269.716751</v>
+        <v>7122283047.92485</v>
       </c>
     </row>
     <row r="401">
@@ -3635,7 +3635,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="n">
-        <v>7194705520.296288</v>
+        <v>7177319567.289192</v>
       </c>
     </row>
     <row r="402">
@@ -3643,7 +3643,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="n">
-        <v>7265138114.080591</v>
+        <v>7214913420.810578</v>
       </c>
     </row>
     <row r="403">
@@ -3651,7 +3651,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="n">
-        <v>7286674797.217772</v>
+        <v>7179302844.735911</v>
       </c>
     </row>
     <row r="404">
@@ -3659,7 +3659,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="n">
-        <v>7309558028.787487</v>
+        <v>7119885561.510461</v>
       </c>
     </row>
     <row r="405">
@@ -3667,7 +3667,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="n">
-        <v>7333625872.942238</v>
+        <v>7039412945.551264</v>
       </c>
     </row>
     <row r="406">
@@ -3675,7 +3675,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="n">
-        <v>7358727803.591136</v>
+        <v>6942836515.30514</v>
       </c>
     </row>
     <row r="407">
@@ -3683,7 +3683,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="n">
-        <v>7384724935.456278</v>
+        <v>6835867090.717943</v>
       </c>
     </row>
     <row r="408">
@@ -3691,7 +3691,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="n">
-        <v>7411489733.808311</v>
+        <v>6723982700.740104</v>
       </c>
     </row>
     <row r="409">
@@ -3699,7 +3699,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="n">
-        <v>7438635531.324885</v>
+        <v>6611887503.406812</v>
       </c>
     </row>
     <row r="410">
@@ -3707,7 +3707,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="n">
-        <v>7463048950.560274</v>
+        <v>6503297952.465577</v>
       </c>
     </row>
     <row r="411">
@@ -3715,7 +3715,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="n">
-        <v>7477000949.988462</v>
+        <v>6400941737.380041</v>
       </c>
     </row>
     <row r="412">
@@ -3723,7 +3723,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="n">
-        <v>7471590089.167496</v>
+        <v>6306663910.659535</v>
       </c>
     </row>
     <row r="413">
@@ -3731,7 +3731,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="n">
-        <v>7446715873.727329</v>
+        <v>6226900408.05384</v>
       </c>
     </row>
     <row r="414">
@@ -3739,7 +3739,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="n">
-        <v>7395326686.490252</v>
+        <v>6156399150.210821</v>
       </c>
     </row>
     <row r="415">
@@ -3747,7 +3747,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="n">
-        <v>7320318683.095544</v>
+        <v>6095453220.726263</v>
       </c>
     </row>
     <row r="416">
@@ -3755,7 +3755,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="n">
-        <v>7226854987.615487</v>
+        <v>6043934733.82719</v>
       </c>
     </row>
     <row r="417">
@@ -3763,7 +3763,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="n">
-        <v>7120971489.480902</v>
+        <v>6001501779.171216</v>
       </c>
     </row>
     <row r="418">
@@ -3771,7 +3771,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="n">
-        <v>7008525584.308103</v>
+        <v>5967668203.145183</v>
       </c>
     </row>
     <row r="419">
@@ -3779,7 +3779,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="n">
-        <v>6894608581.684832</v>
+        <v>5941863889.382259</v>
       </c>
     </row>
     <row r="420">
@@ -3787,7 +3787,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="n">
-        <v>6783301054.023486</v>
+        <v>5923476633.070975</v>
       </c>
     </row>
     <row r="421">
@@ -3795,7 +3795,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="n">
-        <v>6677652867.649948</v>
+        <v>5911881546.791869</v>
       </c>
     </row>
     <row r="422">
@@ -3803,7 +3803,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="n">
-        <v>6579781838.597934</v>
+        <v>5906461178.366602</v>
       </c>
     </row>
     <row r="423">
@@ -3811,7 +3811,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="n">
-        <v>6491021481.509317</v>
+        <v>5906623940.133273</v>
       </c>
     </row>
     <row r="424">
@@ -3819,7 +3819,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="n">
-        <v>6412082848.911379</v>
+        <v>5911808706.587501</v>
       </c>
     </row>
     <row r="425">
@@ -3827,7 +3827,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="n">
-        <v>6343204240.97395</v>
+        <v>5921493121.67183</v>
       </c>
     </row>
     <row r="426">
@@ -3835,7 +3835,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="n">
-        <v>6284277192.307915</v>
+        <v>5935192967.46286</v>
       </c>
     </row>
     <row r="427">
@@ -3843,7 +3843,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="n">
-        <v>6234954532.377482</v>
+        <v>5952465485.228136</v>
       </c>
     </row>
     <row r="428">
@@ -3851,7 +3851,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="n">
-        <v>6194728869.561456</v>
+        <v>5972908155.288429</v>
       </c>
     </row>
     <row r="429">
@@ -3859,7 +3859,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="n">
-        <v>6162998184.366898</v>
+        <v>5996153108.414503</v>
       </c>
     </row>
     <row r="430">
@@ -3867,7 +3867,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="n">
-        <v>6139113609.079107</v>
+        <v>6021872597.214459</v>
       </c>
     </row>
     <row r="431">
@@ -3875,7 +3875,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="n">
-        <v>6122408578.419415</v>
+        <v>6049767730.21934</v>
       </c>
     </row>
     <row r="432">
@@ -3883,7 +3883,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="n">
-        <v>6112227086.164994</v>
+        <v>6079571377.137163</v>
       </c>
     </row>
     <row r="433">
@@ -3891,7 +3891,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="n">
-        <v>6107937472.387991</v>
+        <v>6111044314.271119</v>
       </c>
     </row>
     <row r="434">
@@ -3899,7 +3899,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="n">
-        <v>6108941746.040624</v>
+        <v>6143973095.169992</v>
       </c>
     </row>
     <row r="435">
@@ -3907,7 +3907,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="n">
-        <v>6114681883.244496</v>
+        <v>6178166027.236353</v>
       </c>
     </row>
     <row r="436">
@@ -3915,7 +3915,7 @@
         <v>434</v>
       </c>
       <c r="B436" t="n">
-        <v>6124642751.328428</v>
+        <v>6213452486.520901</v>
       </c>
     </row>
     <row r="437">
@@ -3923,7 +3923,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="n">
-        <v>6138352223.65941</v>
+        <v>6249679939.921967</v>
       </c>
     </row>
     <row r="438">
@@ -3931,7 +3931,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="n">
-        <v>6155382888.145127</v>
+        <v>6286713649.152711</v>
       </c>
     </row>
     <row r="439">
@@ -3939,7 +3939,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="n">
-        <v>6175346028.098156</v>
+        <v>6324431944.96664</v>
       </c>
     </row>
     <row r="440">
@@ -3947,7 +3947,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="n">
-        <v>6197891370.756292</v>
+        <v>6362728717.233105</v>
       </c>
     </row>
     <row r="441">
@@ -3955,7 +3955,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="n">
-        <v>6222704642.063269</v>
+        <v>6401507814.329072</v>
       </c>
     </row>
     <row r="442">
@@ -3963,7 +3963,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="n">
-        <v>6249504498.917107</v>
+        <v>6440684562.732122</v>
       </c>
     </row>
     <row r="443">
@@ -3971,7 +3971,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="n">
-        <v>6278039658.864559</v>
+        <v>6480182477.723499</v>
       </c>
     </row>
     <row r="444">
@@ -3979,7 +3979,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="n">
-        <v>6308084963.259822</v>
+        <v>6519935158.968338</v>
       </c>
     </row>
     <row r="445">
@@ -3987,7 +3987,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="n">
-        <v>6339442615.708363</v>
+        <v>6559882670.298744</v>
       </c>
     </row>
     <row r="446">
@@ -3995,7 +3995,7 @@
         <v>444</v>
       </c>
       <c r="B446" t="n">
-        <v>6371934057.521714</v>
+        <v>6599971980.649581</v>
       </c>
     </row>
     <row r="447">
@@ -4003,7 +4003,7 @@
         <v>445</v>
       </c>
       <c r="B447" t="n">
-        <v>6405401063.101701</v>
+        <v>6640156546.353209</v>
       </c>
     </row>
     <row r="448">
@@ -4011,7 +4011,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="n">
-        <v>6439704626.585558</v>
+        <v>6680394699.97132</v>
       </c>
     </row>
     <row r="449">
@@ -4019,7 +4019,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="n">
-        <v>6474721609.786341</v>
+        <v>6720649451.120564</v>
       </c>
     </row>
     <row r="450">
@@ -4027,7 +4027,7 @@
         <v>448</v>
       </c>
       <c r="B450" t="n">
-        <v>6510341671.382528</v>
+        <v>6760889159.400339</v>
       </c>
     </row>
     <row r="451">
@@ -4035,7 +4035,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="n">
-        <v>6546468581.740669</v>
+        <v>6801083954.396004</v>
       </c>
     </row>
     <row r="452">
@@ -4043,7 +4043,7 @@
         <v>450</v>
       </c>
       <c r="B452" t="n">
-        <v>88644756.05736068</v>
+        <v>88705264.45736068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>